<commit_message>
Added notebook 5 and updated Netherlands annotations
</commit_message>
<xml_diff>
--- a/data/5-annotations/annotations.xlsx
+++ b/data/5-annotations/annotations.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28618"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10112"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32CB06F9-64C1-42E0-84B8-FA135ADC1FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/betzabe/Desktop/MPA_Year_2/Capstone/UKHSA-Capstone/data/5-annotations/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6E001A-E4B5-F84C-8CB3-DEA8F568F62A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="19">
   <si>
     <t>country</t>
   </si>
@@ -69,6 +74,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>periodic*</t>
@@ -78,6 +84,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> progress reporting" (?). In Chile it not too obvious the progress reporting (no include the frequency), but it has.</t>
@@ -104,91 +111,6 @@
   </si>
   <si>
     <t>netherlands</t>
-  </si>
-  <si>
-    <t>Actors agree to the following goals: The number of avoidable healthcare-associated infections 10 will be reduced by 50% in five years, compared with a baseline defined by the relevant actors. During the next five years, the objective is to achieve a reduction of at least 50% in the use of incorrectly prescribed antibiotics across the entire
-healthcare chain</t>
-  </si>
-  <si>
-    <t>The reduction of antibiotic use has flattened. Our current goal focuses on a 70%
-reduction compared with 2009. The sectors and veterinarians will need to do
-everything in their power to further reduce antibiotic use. In order to achieve a
-further reduction, effort is needed specifically on: Additional measures by sectors/veterinarians and strong continuation of implementation of the current policy. The large animal farming sectors face the challenge of stimulating farmers and veterinarians in the 'action area' (red) and the 'warning area' (orange) to shift towards the 'target area' (green) of restrained and prudent antibiotic use. The sectors and veterinarians have already prepared additional measures that will be executed in 2015.
-· Prudent and restricted use in other animal sectors (pets, horses, rabbits, etc.)
-along with reduction of critical antibiotic use in these sectors to this end. We
-will develop an approach in 2015.
-· Continuation of more stringent NVWA (the Netherlands Food and Consumer
-Product Safety Authority) inspections and enforcement of restricted antibiotic
-use in animal farming and identification and control of illegal activities.
-· Improvement of general animal health in order to achieve extremely restricted
-antibiotic use. This is a crucial challenge for actors in the chain, sectors and
-individual animal farmers, in consultation with their veterinarians. It is
-important that restricted and prudent antibiotic use is linked to the innovation
-and sustainability agendas of all the chains affected.</t>
-  </si>
-  <si>
-    <t>Despite these uncertainties, the research by ZonMw and the recommendations by
-the RIVM show that the environment does play a role in the transmission of
-antibiotic resistance. This outcome provides ample reason to initiate a number of
-activities.
-1. We will ask the RIVM to draft an action plan for gaining better insight into the
-situation in the Netherlands. Where necessary, the RIVM will involve other
-actors (e.g. veterinary institutions/experts). This action plan must result in an
-advisory report on the most effective management measures by mid 2016. At
-the very least, the implementation of the action plan must encompass
-measurement of the occurrence of resistant bacteria and the presence of
-(traces of) antibiotics in the environment. To this end, measurements will be
-performed in waste water from health facilities and residential areas, in waste
-water treatment plants and in manure, among other places. The research will
-begin soon. Besides, the Ministry of Economic Affairs has commissioned
-research into the presence of antibiotic residues in manure. The studies will be
-harmonised.
-2. Additionally, antibiotic resistance will be included in a number ofinitiatives,
-such as the Green Deal sustainable operations in healthcare15 and in the new
-water quality policy.</t>
-  </si>
-  <si>
-    <t>We will regularly inform Parliament of the progress of the approach to antibiotic
-resistance. We propose to send an initial progress report in late December 2015.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of avoidable healthcare-associated infections 10 will be reduced by 50% in five years, compared with a baseline defined by the relevant actors. </t>
-  </si>
-  <si>
-    <t>For professionals, the strategy consists of sharing knowledge and stimulating
-new developments. Additionally, there will be more focus on reminding
-professionals of the sense of urgency, placing it higher on the agenda.
-Suggested courses of action will also be offered within the professional field,
-for example in the domain of hygiene.</t>
-  </si>
-  <si>
-    <t>This strategy includes:
-· Increasing public awareness of the problem and increasing knowledge about
-how antibiotics work and should be used. A national campaign must raise
-public awareness and give people more knowledge on which to base their own
-choices. The campaign will provide simple, concrete tips for prevention. The
-communication efforts will use existing instruments and channels wherever
-possible, and new tools will be developed as needed. Additionally,
-communication will be carried out by parties close to the public, such as GPs
-and pharmacists, supported by the necessary campaign materials.</t>
-  </si>
-  <si>
-    <t>Additionally, the National Institute for Public Health and the Environment (RIVM)
-was recently appointed as WHO Collaborating Centre for Antimicrobial Resistance
-Epidemiology and Surveillance. This means the RIVM provides technical support to
-WHO member states in creating and strengthening surveillance of resistant
-bacteria, following the Dutch model. Attention is also given to antibiotic resistance
-in developing nations via Dutch support for the Global Fund for AIDS, Tuberculosis
-and Malaria, with a particular focus on multiresistant tuberculosis.</t>
-  </si>
-  <si>
-    <t>Providing concrete advice on the prevention of bacterial infections. Themes
-include food safety, hygiene, transmission of (resistant) bacteria via pets and
-the importance of following instructions about the use of antibiotics and
-hygiene guidelines.                                                                                                                                                                 Early detection of and swift response to resistant bacteria and other infectious
-threats ensure that the number of carriers9 of resistant bacteria and the
-number of infections and deaths due to antibiotic resistance in the Netherlands
-will remain at the current level or decrease</t>
   </si>
   <si>
     <t>During the next five years, the objective is to achieve a reduction of at least
@@ -202,27 +124,18 @@
 taken into consideration.</t>
   </si>
   <si>
-    <t xml:space="preserve">We support the development of international fundamental scientific knowledge
-by commissioning a new assignment to The Netherlands Organisation for
-Health Research and Development (ZonMW) and by supporting permanent
-participation in the European Joint Programming Initiative on antimicrobial
-resistance. This programme strives for better cooperation between EU
-member states (but also partner nations such as Canada) in the field of
-research in order to harmonise national research programmes and jointly
-initiate and fund expensive and complex research.                                                                                        We support and cooperate in international initiatives designed to develop new
-business models. An existing example is the project 'DRIVE-AB’, which is
-funded via the European Innovative Medicines Initiative and is also part of the
-WHO Global Action Plan on antimicrobial resistance. Together with other
-countries, the WHO and NGOs, we examine whether developments and good
-use of new medicines can be stimulated via a public-private initiative, as is
-currently the case for poverty-related diseases. </t>
+    <t>"For professionals, the strategy consists of sharing knowledge and stimulating
+new developments. Additionally, there will be more focus on reminding
+professionals of the sense of urgency, placing it higher on the agenda.
+Suggested courses of action will also be offered within the professional field,
+for example in the domain of hygiene."</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,6 +162,7 @@
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -256,6 +170,7 @@
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -278,6 +193,13 @@
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -309,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -340,6 +262,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -678,21 +603,21 @@
   <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B65" sqref="B65:B66"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="14.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="3" customWidth="1"/>
     <col min="4" max="4" width="56" style="3" customWidth="1"/>
-    <col min="5" max="5" width="80.42578125" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="3"/>
+    <col min="5" max="5" width="80.5" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -709,7 +634,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -720,7 +645,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -731,7 +656,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -742,7 +667,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -753,7 +678,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -764,7 +689,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -775,7 +700,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="38.25">
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -790,7 +715,7 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -801,7 +726,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -812,7 +737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
@@ -823,7 +748,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>5</v>
       </c>
@@ -834,7 +759,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>5</v>
       </c>
@@ -845,7 +770,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="63">
+    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
@@ -860,7 +785,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>5</v>
       </c>
@@ -871,7 +796,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
@@ -882,7 +807,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>5</v>
       </c>
@@ -893,7 +818,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>5</v>
       </c>
@@ -907,7 +832,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>5</v>
       </c>
@@ -918,7 +843,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>5</v>
       </c>
@@ -929,7 +854,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>5</v>
       </c>
@@ -940,7 +865,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="38.25">
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>5</v>
       </c>
@@ -957,7 +882,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>14</v>
       </c>
@@ -965,7 +890,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>14</v>
       </c>
@@ -973,7 +898,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>14</v>
       </c>
@@ -981,7 +906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>14</v>
       </c>
@@ -989,7 +914,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>14</v>
       </c>
@@ -997,7 +922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>14</v>
       </c>
@@ -1005,7 +930,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>14</v>
       </c>
@@ -1013,7 +938,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>14</v>
       </c>
@@ -1021,7 +946,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>14</v>
       </c>
@@ -1029,7 +954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>14</v>
       </c>
@@ -1037,7 +962,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>14</v>
       </c>
@@ -1045,7 +970,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>14</v>
       </c>
@@ -1053,7 +978,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>14</v>
       </c>
@@ -1061,7 +986,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>14</v>
       </c>
@@ -1069,7 +994,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>14</v>
       </c>
@@ -1077,7 +1002,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>14</v>
       </c>
@@ -1085,7 +1010,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>14</v>
       </c>
@@ -1093,7 +1018,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>14</v>
       </c>
@@ -1101,7 +1026,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>14</v>
       </c>
@@ -1109,7 +1034,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>14</v>
       </c>
@@ -1117,7 +1042,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>14</v>
       </c>
@@ -1125,7 +1050,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>15</v>
       </c>
@@ -1136,7 +1061,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>15</v>
       </c>
@@ -1147,7 +1072,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>15</v>
       </c>
@@ -1158,7 +1083,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>15</v>
       </c>
@@ -1169,7 +1094,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>15</v>
       </c>
@@ -1180,7 +1105,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>15</v>
       </c>
@@ -1191,7 +1116,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>15</v>
       </c>
@@ -1202,7 +1127,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>15</v>
       </c>
@@ -1213,7 +1138,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>15</v>
       </c>
@@ -1224,7 +1149,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>15</v>
       </c>
@@ -1235,7 +1160,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>15</v>
       </c>
@@ -1246,7 +1171,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>15</v>
       </c>
@@ -1257,7 +1182,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>15</v>
       </c>
@@ -1268,7 +1193,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>15</v>
       </c>
@@ -1279,7 +1204,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>15</v>
       </c>
@@ -1290,7 +1215,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>15</v>
       </c>
@@ -1301,7 +1226,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>15</v>
       </c>
@@ -1312,7 +1237,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>15</v>
       </c>
@@ -1323,7 +1248,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>15</v>
       </c>
@@ -1334,7 +1259,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>15</v>
       </c>
@@ -1345,7 +1270,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>15</v>
       </c>
@@ -1356,7 +1281,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>16</v>
       </c>
@@ -1367,7 +1292,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>16</v>
       </c>
@@ -1378,255 +1303,237 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="105.75" customHeight="1">
+    <row r="67" spans="1:5" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B67" s="3">
         <v>1</v>
       </c>
-      <c r="C67" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E67" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="240">
+      <c r="C67" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" s="10"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B68" s="3">
         <v>2</v>
       </c>
-      <c r="C68" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E68" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="240">
+      <c r="C68" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" s="10"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B69" s="3">
         <v>3</v>
       </c>
-      <c r="C69" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E69" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="C69" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" s="10"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B70" s="3">
         <v>4</v>
       </c>
-      <c r="C70" s="9" t="s">
-        <v>10</v>
+      <c r="C70" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="E70" s="10"/>
     </row>
-    <row r="71" spans="1:5" ht="25.5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B71" s="3">
         <v>5</v>
       </c>
-      <c r="C71" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E71" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="25.5">
+      <c r="C71" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E71" s="10"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B72" s="3">
         <v>6</v>
       </c>
-      <c r="C72" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E72" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
+      <c r="C72" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E72" s="10"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B73" s="3">
         <v>7</v>
       </c>
-      <c r="C73" s="9" t="s">
+      <c r="C73" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E73" s="9"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B74" s="3">
         <v>8</v>
       </c>
-      <c r="C74" s="9" t="s">
+      <c r="C74" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E74" s="9"/>
     </row>
-    <row r="75" spans="1:5" ht="63">
+    <row r="75" spans="1:5" ht="75" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B75" s="3">
         <v>9</v>
       </c>
-      <c r="C75" s="9" t="s">
+      <c r="C75" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E75" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="113.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B76" s="3">
         <v>10</v>
       </c>
-      <c r="C76" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E76" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="88.5">
+      <c r="C76" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76" s="10"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B77" s="3">
         <v>11</v>
       </c>
-      <c r="C77" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E77" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
+      <c r="C77" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" s="10"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B78" s="3">
         <v>12</v>
       </c>
-      <c r="C78" s="9" t="s">
+      <c r="C78" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E78" s="9"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B79" s="3">
         <v>13</v>
       </c>
-      <c r="C79" s="9" t="s">
+      <c r="C79" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E79" s="9"/>
     </row>
-    <row r="80" spans="1:5" ht="100.5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B80" s="3">
         <v>14</v>
       </c>
-      <c r="C80" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E80" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5">
+      <c r="C80" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E80" s="10"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B81" s="3">
         <v>15</v>
       </c>
-      <c r="C81" s="9" t="s">
+      <c r="C81" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E81" s="9"/>
     </row>
-    <row r="82" spans="1:5" ht="113.25">
+    <row r="82" spans="1:5" ht="135" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B82" s="3">
         <v>16</v>
       </c>
-      <c r="C82" s="9" t="s">
+      <c r="C82" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E82" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B83" s="3">
         <v>17</v>
       </c>
-      <c r="C83" s="9" t="s">
+      <c r="C83" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E83" s="9"/>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B84" s="3">
         <v>18</v>
       </c>
-      <c r="C84" s="9" t="s">
+      <c r="C84" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E84" s="9"/>
     </row>
-    <row r="85" spans="1:5" ht="189">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B85" s="3">
         <v>19</v>
       </c>
-      <c r="C85" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E85" s="10" t="s">
-        <v>27</v>
-      </c>
+      <c r="C85" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E85" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>